<commit_message>
modified and adding all working cascaded testcases given by Raj.
</commit_message>
<xml_diff>
--- a/ScenarioBuilder/roostify-test-configuration.xlsx
+++ b/ScenarioBuilder/roostify-test-configuration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
   <si>
     <t>Test Suite</t>
   </si>
@@ -165,16 +165,70 @@
     <t>https://scenariobuilder-test.herokuapp.com/</t>
   </si>
   <si>
-    <t>selected</t>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-06-59-checkEnablingOfGetMyOptionsButton.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-07-18-validateGraphLegends.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-07-32-validateOptionsForPurchase.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-07-36-validateOptionsForRefinance.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-07-51-validateOptionsForRefinanceCashout.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-08-05-validateOtherOptimizations.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-08-08-validateZipCodeError.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-08-11-validateZipCodeLookUp.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-08-25-validatingLeadForm.png</t>
   </si>
   <si>
     <t>smoke</t>
   </si>
   <si>
-    <t>C:\Users\E6430\Desktop\GitHub\workcode\ScenarioBuilder/src/test/resources/screenshots/07-11-2017_16-42-27-validateOptionsForPurchase.png</t>
-  </si>
-  <si>
-    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/07-11-2017_19-56-13-validateOptionsForPurchase.png</t>
+    <t>all</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-17-49-checkEnablingOfGetMyOptionsButton.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-18-06-validateGraphLegends.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-18-20-validateOptionsForPurchase.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-18-25-validateOptionsForRefinance.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-18-40-validateOptionsForRefinanceCashout.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-18-55-validateOtherOptimizations.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-18-57-validateZipCodeError.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-19-01-validateZipCodeLookUp.png</t>
+  </si>
+  <si>
+    <t>C:\Users\E6430\Desktop\GitHubWork\workcode\ScenarioBuilder/src/test/resources/screenshots/09-11-2017_15-19-15-validatingLeadForm.png</t>
   </si>
 </sst>
 </file>
@@ -182,7 +236,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,13 +260,43 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color indexed="13"/>
+      <color indexed="10"/>
       <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color indexed="13"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
       <b val="true"/>
     </font>
     <font>
@@ -222,7 +306,7 @@
       <b val="true"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,7 +324,12 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="lightDown">
+        <bgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightDown">
         <bgColor indexed="17"/>
       </patternFill>
     </fill>
@@ -250,18 +339,8 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="lightDown">
-        <bgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill>
-        <bgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightDown">
-        <bgColor indexed="13"/>
+        <bgColor indexed="17"/>
       </patternFill>
     </fill>
   </fills>
@@ -281,21 +360,39 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -594,7 +691,7 @@
   <dimension ref="A1:AL9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -674,7 +771,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -682,12 +779,15 @@
         <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:38">
       <c r="A9" t="s">
         <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -707,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -768,11 +868,11 @@
       <c r="F2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="19" t="s">
         <v>34</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -794,8 +894,12 @@
       <c r="F3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
@@ -816,8 +920,12 @@
       <c r="F4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
+      <c r="G4" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
@@ -836,8 +944,12 @@
         <v>40</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
@@ -856,8 +968,12 @@
         <v>46</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="4"/>
+      <c r="G6" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
@@ -876,8 +992,12 @@
         <v>41</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
@@ -896,8 +1016,12 @@
         <v>46</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="4"/>
+      <c r="G8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
@@ -916,8 +1040,12 @@
         <v>41</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
@@ -936,8 +1064,12 @@
         <v>46</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="4"/>
+      <c r="G10" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>